<commit_message>
Adding Screenshot methods. Code improvisation.
</commit_message>
<xml_diff>
--- a/src/resources/data/DataSheet.xlsx
+++ b/src/resources/data/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0" date1904="1" showInkAnnotation="0"/>
   <bookViews>
-    <workbookView tabRatio="500" windowHeight="18380" windowWidth="25600" xWindow="0" yWindow="0"/>
+    <workbookView tabRatio="500" windowHeight="18380" windowWidth="25600" xWindow="2760" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="SmokeTests" r:id="rId1" sheetId="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="16">
   <si>
     <t>testCase</t>
   </si>
@@ -57,10 +57,16 @@
     <t>failingTestCase</t>
   </si>
   <si>
-    <t>₹69,990</t>
-  </si>
-  <si>
-    <t>65 inch 4K UHD ANDROID SMART SAMSUNG PANEL 8GB LED TV +REPLACEMENT WARRANTY</t>
+    <t>₹153,799</t>
+  </si>
+  <si>
+    <t>SONY 65 INCHES 65X7000E 4k UHD HDR SMART LED TV + ONE YEAR DEALER'S WARRANTY</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Rs.153,799</t>
   </si>
 </sst>
 </file>
@@ -468,7 +474,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -500,7 +506,9 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
@@ -519,7 +527,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -544,7 +552,6 @@
     <hyperlink r:id="rId2" ref="B3"/>
   </hyperlinks>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup horizontalDpi="4294967292" orientation="portrait" paperSize="9" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>